<commit_message>
Working cards without filters
</commit_message>
<xml_diff>
--- a/GD.codexalgorithm_contents_sheet.xlsx
+++ b/GD.codexalgorithm_contents_sheet.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="55">
   <si>
     <t>Timestamp</t>
   </si>
@@ -302,6 +302,33 @@
   </si>
   <si>
     <t>https://drive.google.com/open?id=1CtGaGOexFIC5nTXrT3vWrVKbOF5SNIyM</t>
+  </si>
+  <si>
+    <t>Test enty</t>
+  </si>
+  <si>
+    <t>Test entry text</t>
+  </si>
+  <si>
+    <t>Machine learning</t>
+  </si>
+  <si>
+    <t>Neural network</t>
+  </si>
+  <si>
+    <t>AI that creates</t>
+  </si>
+  <si>
+    <t>Real-time rendering</t>
+  </si>
+  <si>
+    <t>Learning</t>
+  </si>
+  <si>
+    <t>Simulation</t>
+  </si>
+  <si>
+    <t>Is run locally, Runs on PC, Runs on Playstation, Runs on handheld devices</t>
   </si>
 </sst>
 </file>
@@ -471,10 +498,10 @@
         <color rgb="FF442F65"/>
       </left>
       <right style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </right>
       <top style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </top>
       <bottom style="thin">
         <color rgb="FF442F65"/>
@@ -482,13 +509,13 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </left>
       <right style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </right>
       <top style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </top>
       <bottom style="thin">
         <color rgb="FF442F65"/>
@@ -498,7 +525,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -508,6 +535,9 @@
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
@@ -538,13 +568,13 @@
     <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="9" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -605,7 +635,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:Q6" displayName="Form_Responses1" name="Form_Responses1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:Q7" displayName="Form_Responses1" name="Form_Responses1" id="1">
   <tableColumns count="17">
     <tableColumn name="Timestamp" id="1"/>
     <tableColumn name="System name" id="2"/>
@@ -860,294 +890,335 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4">
+      <c r="A2" s="5">
         <v>45660.62919707176</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="5">
+      <c r="L2" s="6">
         <v>6.0</v>
       </c>
-      <c r="M2" s="5">
+      <c r="M2" s="6">
         <v>1.0</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="O2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="Q2" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="8">
+      <c r="A3" s="9">
         <v>45661.68384380787</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="9">
+      <c r="L3" s="10">
         <v>6.0</v>
       </c>
-      <c r="M3" s="9">
+      <c r="M3" s="10">
         <v>1.0</v>
       </c>
-      <c r="N3" s="9" t="s">
+      <c r="N3" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="P3" s="9" t="s">
+      <c r="P3" s="10" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="10">
+      <c r="A4" s="11">
         <v>45661.690393275465</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="11">
+      <c r="L4" s="12">
         <v>6.0</v>
       </c>
-      <c r="M4" s="11">
+      <c r="M4" s="12">
         <v>1.0</v>
       </c>
-      <c r="N4" s="11" t="s">
+      <c r="N4" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="P4" s="11" t="s">
+      <c r="P4" s="12" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="8">
+      <c r="A5" s="9">
         <v>45661.69956625</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="J5" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="K5" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="L5" s="9">
+      <c r="L5" s="10">
         <v>6.0</v>
       </c>
-      <c r="M5" s="9">
+      <c r="M5" s="10">
         <v>1.0</v>
       </c>
-      <c r="N5" s="9" t="s">
+      <c r="N5" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="P5" s="12" t="s">
+      <c r="P5" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="13">
+      <c r="A6" s="11">
         <v>45661.70633385416</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="J6" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="K6" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L6" s="12">
         <v>6.0</v>
       </c>
-      <c r="M6" s="14">
+      <c r="M6" s="12">
         <v>1.0</v>
       </c>
-      <c r="N6" s="14" t="s">
+      <c r="N6" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="O6" s="15" t="s">
+      <c r="O6" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="P6" s="14" t="s">
+      <c r="P6" s="12" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="15">
+        <v>45672.671838738424</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="L7" s="16">
+        <v>4.0</v>
+      </c>
+      <c r="M7" s="16">
+        <v>8.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>